<commit_message>
Electronics BOM various update
</commit_message>
<xml_diff>
--- a/bom/BOM_Electronics.xlsx
+++ b/bom/BOM_Electronics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FE85F4-9F33-4E1F-BAB0-8E9B44ABA22E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A226B76-504E-4DF1-8DB5-1E24A245967B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{1A685599-6F45-4184-BD49-3F7235A0E362}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1A685599-6F45-4184-BD49-3F7235A0E362}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="106">
   <si>
     <t>SubAssy</t>
   </si>
@@ -113,10 +113,6 @@
   </si>
   <si>
     <t xml:space="preserve">25 Amp Solid State Relay.  3 - 32VDC input, 24-380VAC control </t>
-  </si>
-  <si>
-    <t>Required to drive the recommended bed heat pad which uses mains power (110Vac or 220Vac). 
-The solid state will source power from the mains and distribute to the bed as instructed by the conrol board.</t>
   </si>
   <si>
     <t>Amazon
@@ -211,10 +207,6 @@
     <t>https://duet3d.com/Duet3Mainboard6HC</t>
   </si>
   <si>
-    <t>Duet 3 has 6 independent stepper driver, which is enough to control all basis stepper from the HevORT:
-X, Y, Z, Z, Z and E</t>
-  </si>
-  <si>
     <t>B2</t>
   </si>
   <si>
@@ -230,9 +222,6 @@
     <t>OPTION B</t>
   </si>
   <si>
-    <t>Duet3</t>
-  </si>
-  <si>
     <t>Duet2 + Duex5</t>
   </si>
   <si>
@@ -245,13 +234,7 @@
     <t>110VAC or 220VAC Silicone Heater pad</t>
   </si>
   <si>
-    <t>*Dimension defined in Frame Calculator: https://miragec79.github.io/HevORT/framecalculator.html</t>
-  </si>
-  <si>
     <t>AliExpress</t>
-  </si>
-  <si>
-    <t>https://keenovo.aliexpress.com/store/210086?spm=a2g0o.productlist.0.0.184c4ec1syswHe</t>
   </si>
   <si>
     <t>Keenovo Silicon Heat Pad using AC mains voltage</t>
@@ -311,15 +294,9 @@
     <t>One kit is plenty, you may want to buy less, but I always like to have wire spool readily available when rewuired.</t>
   </si>
   <si>
-    <t>https://amzn.to/3gGWO9t</t>
-  </si>
-  <si>
     <t>https://amzn.to/2IAQVhq</t>
   </si>
   <si>
-    <t>https://amzn.to/2W03pCf</t>
-  </si>
-  <si>
     <t>General Wires for component connection</t>
   </si>
   <si>
@@ -332,17 +309,117 @@
     <t>https://amzn.to/3oIbW9u</t>
   </si>
   <si>
-    <t>https://amzn.to/3gCo6xM</t>
-  </si>
-  <si>
-    <t>https://amzn.to/344o64q</t>
+    <r>
+      <t xml:space="preserve">Required to drive the recommended bed heat pad which uses mains power (110Vac or 220Vac). 
+The solid state will source power from the mains and distribute to the bed as instructed by the conrol board.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>***CAREFULL***  many sources claim they sell genuine Fotek. Know hoe to spot the difference: https://protosupplies.com/inferior-counterfeit-fotek-ssr-25-solid-state-relays-on-the-market/</t>
+    </r>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_AtyIW2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">300X300: https://s.click.aliexpress.com/e/_9yE4CA
+400X400: https://s.click.aliexpress.com/e/_99UVxg
+** 500X500: https://s.click.aliexpress.com/e/_A7JDf0
+</t>
+  </si>
+  <si>
+    <t>*Dimension defined in Frame Calculator: https://miragec79.github.io/HevORT/framecalculator.html
+**Verify with you house power grid capacity as some 500mm heaters might exceed the limit of a single breaker.</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_A8RohY</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Duet 3 has 6 independent stepper driver, which is enough to control all basis stepper from the HevORT:
+X, Y, Z, Z, Z and E
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>As of Now Klipper is not supported on the Duet3 6HC board.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Duet3 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>( DOES NOT SUPPORT KLIPPER YET)</t>
+    </r>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_AlBj54</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_Ad1dVk</t>
+  </si>
+  <si>
+    <t>OPTION C</t>
+  </si>
+  <si>
+    <t>Single board computer for Klipper</t>
+  </si>
+  <si>
+    <t>OPTIONAL</t>
+  </si>
+  <si>
+    <t>*Optional
+Although you do not absolutely require a raspberry pi to get your Duet2 running, the RPI will enable you to run Klipper Firmware instead of RRF.
+Read more about Klipper: https://www.klipper3d.org/</t>
+  </si>
+  <si>
+    <t>Other Popular Boards (Recommended to use Klipper Firmware with these boards)</t>
+  </si>
+  <si>
+    <t>*Optional
+Although you do not absolutely require a raspberry pi to get your control board running, the RPI will enable you to run Klipper Firmware instead of RRF or Marlin.
+Read more about Klipper: https://www.klipper3d.org/</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>https://s.click.aliexpress.com/e/_9hfn54</t>
+  </si>
+  <si>
+    <t>Fysetc S6 Spider V1.1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,6 +534,21 @@
       <u/>
       <sz val="12"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -606,7 +698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -730,6 +822,15 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1122,8 +1223,8 @@
       <xdr:rowOff>350371</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>1636060</xdr:colOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>1098005</xdr:rowOff>
     </xdr:to>
@@ -1240,13 +1341,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>145679</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>294528</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1459940</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>1179251</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1300,15 +1401,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>358587</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>145676</xdr:rowOff>
+      <xdr:colOff>347381</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>616323</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>1235821</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>998082</xdr:rowOff>
+      <xdr:colOff>1224615</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>1468729</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1338,8 +1439,8 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="3440205" y="10780058"/>
-          <a:ext cx="877234" cy="855581"/>
+          <a:off x="3316940" y="11183470"/>
+          <a:ext cx="877234" cy="852406"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1362,13 +1463,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>372141</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>151334</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1257013</xdr:colOff>
-      <xdr:row>11</xdr:row>
+      <xdr:row>15</xdr:row>
       <xdr:rowOff>1008529</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1423,13 +1524,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>324973</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>140819</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1190998</xdr:colOff>
-      <xdr:row>12</xdr:row>
+      <xdr:row>16</xdr:row>
       <xdr:rowOff>980703</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1484,13 +1585,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>237806</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>163262</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1269439</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>1193441</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1545,13 +1646,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>340562</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>208527</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1277470</xdr:colOff>
-      <xdr:row>14</xdr:row>
+      <xdr:row>18</xdr:row>
       <xdr:rowOff>1149921</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1606,13 +1707,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1654,13 +1755,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>304800</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
@@ -1702,13 +1803,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>276974</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>369795</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1250883</xdr:colOff>
-      <xdr:row>15</xdr:row>
+      <xdr:row>19</xdr:row>
       <xdr:rowOff>1314264</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1763,13 +1864,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>408268</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>118409</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1255059</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>914181</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1824,13 +1925,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>121228</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1437409</xdr:colOff>
-      <xdr:row>5</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>1364339</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1885,13 +1986,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>155864</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>432954</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1514054</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:row>7</xdr:row>
       <xdr:rowOff>1457902</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1946,13 +2047,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>190500</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>238499</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1437528</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>1179436</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2007,13 +2108,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>120090</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>104028</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1552762</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>21</xdr:row>
       <xdr:rowOff>932377</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2068,13 +2169,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>156883</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>134470</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>1583205</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>22</xdr:row>
       <xdr:rowOff>962819</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -2125,12 +2226,185 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>155864</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>432954</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1358190" cy="1024948"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="20" name="Picture 19" descr="See the source image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EEC2B344-CB4F-4CCA-96AB-46E055D04FFA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3125423" y="7145278"/>
+          <a:ext cx="1358190" cy="1024948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>155864</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>432954</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="1358190" cy="1024948"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="22" name="Picture 21" descr="See the source image">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1BB2A00-8423-4F0E-8F7B-A39BEEA8C779}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="3248688" y="7884866"/>
+          <a:ext cx="1358190" cy="1024948"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>295239</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>152997</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1312556</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>2061882</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="26" name="Picture 25">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD5B8800-7E92-4412-A049-7BD6FBCD779F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId16" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm rot="5400000">
+          <a:off x="2942279" y="10437546"/>
+          <a:ext cx="1908885" cy="1017317"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D1A77ADD-644D-4017-B666-BDF7D0FA2682}" name="Table1" displayName="Table1" ref="A1:K19" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10">
-  <autoFilter ref="A1:K19" xr:uid="{9012886B-C279-4CC5-9744-219E58D55D65}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D1A77ADD-644D-4017-B666-BDF7D0FA2682}" name="Table1" displayName="Table1" ref="A1:K23" totalsRowShown="0" headerRowDxfId="11" headerRowBorderDxfId="10">
+  <autoFilter ref="A1:K23" xr:uid="{9012886B-C279-4CC5-9744-219E58D55D65}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{C4F07B76-F79C-478F-972D-DFE1D78494F0}" name="SubAssy" dataDxfId="9"/>
     <tableColumn id="2" xr3:uid="{A12454AA-35A1-414A-9FFC-6C4FBFB03962}" name="Category" dataDxfId="8"/>
@@ -2445,26 +2719,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DA158D-DB07-4293-994E-A3724E044295}">
-  <dimension ref="A1:K19"/>
+  <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.54296875" customWidth="1"/>
-    <col min="2" max="2" width="22.90625" customWidth="1"/>
-    <col min="4" max="4" width="24.54296875" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="27.54296875" customWidth="1"/>
-    <col min="7" max="7" width="17.1796875" customWidth="1"/>
-    <col min="9" max="9" width="56.08984375" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="9" max="9" width="56.140625" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="56.6328125" customWidth="1"/>
+    <col min="11" max="11" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="42.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2499,12 +2774,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="8" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" s="8" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="36" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="37" t="s">
         <v>60</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>63</v>
       </c>
       <c r="C2" s="38"/>
       <c r="D2" s="29"/>
@@ -2516,7 +2791,7 @@
       <c r="J2" s="33"/>
       <c r="K2" s="41"/>
     </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" ht="111.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:11" s="8" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -2524,7 +2799,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="12" t="s">
@@ -2540,7 +2815,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>15</v>
@@ -2549,7 +2824,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" ht="111.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:11" s="8" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
         <v>12</v>
       </c>
@@ -2557,7 +2832,7 @@
         <v>13</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4"/>
       <c r="E4" s="22" t="s">
@@ -2573,7 +2848,7 @@
         <v>1</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>15</v>
@@ -2582,247 +2857,226 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="8" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A5" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B5" s="37" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="28"/>
-      <c r="D5" s="29"/>
-      <c r="E5" s="30"/>
-      <c r="F5" s="30"/>
-      <c r="G5" s="31"/>
-      <c r="H5" s="32"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="34"/>
-      <c r="K5" s="35"/>
+    <row r="5" spans="1:11" s="8" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5"/>
+      <c r="E5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I5" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="J5" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="17" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" ht="111.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="D6"/>
-      <c r="E6" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F6" s="12" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="14">
-        <v>1</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="J6" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>55</v>
-      </c>
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="36" t="s">
+        <v>59</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>93</v>
+      </c>
+      <c r="C6" s="28"/>
+      <c r="D6" s="29"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="33"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="35"/>
     </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" ht="170" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:11" s="8" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D7"/>
       <c r="E7" s="12" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G7" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H7" s="14" t="s">
-        <v>38</v>
+      <c r="H7" s="14">
+        <v>1</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>72</v>
+        <v>92</v>
       </c>
       <c r="J7" s="16" t="s">
-        <v>80</v>
+        <v>15</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>92</v>
+        <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="36" t="s">
-        <v>64</v>
-      </c>
-      <c r="B8" s="27"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
-      <c r="G8" s="31"/>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33"/>
-      <c r="J8" s="34"/>
-      <c r="K8" s="35"/>
+    <row r="8" spans="1:11" s="8" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D8"/>
+      <c r="E8" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K8" s="17" t="s">
+        <v>85</v>
+      </c>
     </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" ht="111.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="21">
-        <v>3</v>
-      </c>
-      <c r="D9"/>
-      <c r="E9" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="G9" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="23">
-        <v>1</v>
-      </c>
-      <c r="I9" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="J9" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K9" s="26" t="s">
-        <v>93</v>
-      </c>
+    <row r="9" spans="1:11" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="36" t="s">
+        <v>96</v>
+      </c>
+      <c r="B9" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="C9" s="28"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="31"/>
+      <c r="H9" s="32"/>
+      <c r="I9" s="33"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="35"/>
     </row>
-    <row r="10" spans="1:11" s="8" customFormat="1" ht="116" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:11" s="8" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B10" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C10" s="11">
-        <v>4</v>
+      <c r="B10" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>103</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="12" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="12" t="s">
-        <v>70</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F10" s="12"/>
       <c r="G10" s="18"/>
-      <c r="H10" s="14" t="s">
-        <v>38</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="16" t="s">
-        <v>68</v>
-      </c>
+      <c r="H10" s="14"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
       <c r="K10" s="17" t="s">
-        <v>69</v>
+        <v>104</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:11" s="8" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C11" s="21">
-        <v>5</v>
-      </c>
-      <c r="E11" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="22" t="s">
-        <v>25</v>
+      <c r="B11" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="D11"/>
+      <c r="E11" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>56</v>
       </c>
       <c r="G11" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="23">
-        <v>1</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K11" s="26" t="s">
-        <v>89</v>
+      <c r="H11" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="15" t="s">
+        <v>101</v>
+      </c>
+      <c r="J11" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K11" s="17" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B12" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="C12" s="11">
-        <v>6</v>
-      </c>
-      <c r="E12" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="22" t="s">
-        <v>29</v>
-      </c>
-      <c r="G12" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H12" s="23">
-        <v>1</v>
-      </c>
-      <c r="I12" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="J12" s="25" t="s">
-        <v>27</v>
-      </c>
-      <c r="K12" s="26" t="s">
-        <v>94</v>
-      </c>
+    <row r="12" spans="1:11" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A12" s="36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="31"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="33"/>
+      <c r="J12" s="34"/>
+      <c r="K12" s="35"/>
     </row>
-    <row r="13" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:11" s="8" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="C13" s="21">
-        <v>7</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D13"/>
       <c r="E13" s="22" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="G13" s="18" t="s">
         <v>11</v>
@@ -2831,225 +3085,359 @@
         <v>1</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="J13" s="25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K13" s="26" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:11" s="8" customFormat="1" ht="116.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B14" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C14" s="11">
+        <v>4</v>
+      </c>
+      <c r="D14"/>
+      <c r="E14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="11">
-        <v>8</v>
-      </c>
-      <c r="E14" s="22" t="s">
-        <v>32</v>
-      </c>
-      <c r="F14" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G14" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" s="23">
-        <v>1</v>
-      </c>
-      <c r="I14" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="J14" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="26" t="s">
-        <v>33</v>
+      <c r="G14" s="18"/>
+      <c r="H14" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="J14" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="K14" s="43" t="s">
+        <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="138.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="C15" s="21">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E15" s="22" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="F15" s="22" t="s">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="G15" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="23" t="s">
-        <v>38</v>
+      <c r="H15" s="23">
+        <v>1</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>77</v>
+        <v>87</v>
       </c>
       <c r="J15" s="25" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="K15" s="26" t="s">
-        <v>39</v>
+        <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="133" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="20" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C16" s="11">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E16" s="22" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="F16" s="22" t="s">
-        <v>42</v>
+        <v>28</v>
       </c>
       <c r="G16" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="23" t="s">
-        <v>38</v>
+      <c r="H16" s="23">
+        <v>1</v>
       </c>
       <c r="I16" s="24" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="J16" s="25" t="s">
-        <v>43</v>
+        <v>26</v>
       </c>
       <c r="K16" s="26" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="19" t="s">
         <v>12</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>40</v>
+        <v>62</v>
       </c>
       <c r="C17" s="21">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="E17" s="22" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G17" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="23" t="s">
-        <v>46</v>
+      <c r="H17" s="23">
+        <v>1</v>
       </c>
       <c r="I17" s="24" t="s">
-        <v>47</v>
+        <v>70</v>
       </c>
       <c r="J17" s="25" t="s">
-        <v>48</v>
+        <v>26</v>
       </c>
       <c r="K17" s="26" t="s">
-        <v>87</v>
+        <v>94</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="81.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:11" ht="126" x14ac:dyDescent="0.25">
       <c r="A18" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="10" t="s">
-        <v>79</v>
+      <c r="B18" s="20" t="s">
+        <v>62</v>
       </c>
       <c r="C18" s="11">
-        <v>12</v>
-      </c>
-      <c r="E18" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="F18" s="12" t="s">
-        <v>90</v>
+        <v>8</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>34</v>
       </c>
       <c r="G18" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="J18" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="K18" s="17" t="s">
-        <v>81</v>
+      <c r="H18" s="23">
+        <v>1</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="J18" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K18" s="26" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:11" ht="138.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="10" t="s">
-        <v>79</v>
-      </c>
-      <c r="C19" s="11">
-        <v>13</v>
-      </c>
-      <c r="E19" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>91</v>
+      <c r="B19" s="20" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="21">
+        <v>9</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="F19" s="22" t="s">
+        <v>35</v>
       </c>
       <c r="G19" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="H19" s="14" t="s">
+      <c r="H19" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="J19" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="132.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="11">
+        <v>10</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="F20" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="J20" s="25" t="s">
+        <v>42</v>
+      </c>
+      <c r="K20" s="26" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="C21" s="21">
+        <v>11</v>
+      </c>
+      <c r="E21" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="F21" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="I21" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="J21" s="25" t="s">
+        <v>47</v>
+      </c>
+      <c r="K21" s="26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="11">
+        <v>12</v>
+      </c>
+      <c r="E22" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="12" t="s">
         <v>83</v>
       </c>
-      <c r="I19" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="J19" s="16" t="s">
+      <c r="G22" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I22" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K22" s="17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="19" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="C23" s="11">
+        <v>13</v>
+      </c>
+      <c r="E23" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="K19" s="17" t="s">
+      <c r="F23" s="12" t="s">
+        <v>84</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>11</v>
+      </c>
+      <c r="H23" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I23" s="15" t="s">
         <v>81</v>
+      </c>
+      <c r="J23" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="K23" s="17" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="K3" r:id="rId1" display="https://duet3d.com/DuetWifi" xr:uid="{F82F4281-3CD9-46EC-9EA8-12A4905EEF04}"/>
-    <hyperlink ref="K10" r:id="rId2" xr:uid="{4C1DCD2D-9D03-4B9C-808E-3E95340D33E0}"/>
-    <hyperlink ref="K18" r:id="rId3" xr:uid="{0337AE39-3709-4D56-9909-04B6A63BD80E}"/>
-    <hyperlink ref="K19" r:id="rId4" xr:uid="{620FB348-31A3-4960-86B6-4CED00D27CA5}"/>
-    <hyperlink ref="K17" r:id="rId5" xr:uid="{77EAC540-B6A7-4DAC-9613-F256823A3940}"/>
-    <hyperlink ref="K15" r:id="rId6" xr:uid="{30A8D214-505F-4AA8-BE9F-13B1E12EADA7}"/>
-    <hyperlink ref="K11" r:id="rId7" xr:uid="{15E7AC38-70D3-4C77-BA6B-5A5E9C6898D3}"/>
+    <hyperlink ref="K22" r:id="rId2" xr:uid="{0337AE39-3709-4D56-9909-04B6A63BD80E}"/>
+    <hyperlink ref="K23" r:id="rId3" xr:uid="{620FB348-31A3-4960-86B6-4CED00D27CA5}"/>
+    <hyperlink ref="K19" r:id="rId4" xr:uid="{30A8D214-505F-4AA8-BE9F-13B1E12EADA7}"/>
+    <hyperlink ref="K13" r:id="rId5" xr:uid="{3A6407ED-523C-449A-BA12-AB8B6D709F5F}"/>
+    <hyperlink ref="K8" r:id="rId6" xr:uid="{A785EA67-C7DD-4758-8477-AA0705C2693D}"/>
+    <hyperlink ref="K15" r:id="rId7" xr:uid="{7A1F4277-1D0C-466F-A1DB-2F5C899DF2F3}"/>
+    <hyperlink ref="K16" r:id="rId8" xr:uid="{9264ACB5-F8D2-4B15-A406-9BBB6AF84E6D}"/>
+    <hyperlink ref="K17" r:id="rId9" xr:uid="{8F628744-EA36-4572-AB75-C7D1D8038295}"/>
+    <hyperlink ref="K20" r:id="rId10" xr:uid="{A9CA0FCF-7C94-4780-BF60-5D84F620EA95}"/>
+    <hyperlink ref="K21" r:id="rId11" xr:uid="{351134BB-2C37-408C-810D-8A1ABE738310}"/>
+    <hyperlink ref="K5" r:id="rId12" xr:uid="{D54CB7AA-26E4-4CE6-B722-81FA3F21507D}"/>
+    <hyperlink ref="K11" r:id="rId13" xr:uid="{21EBD8DB-10FC-4A97-A28E-DC53AEE9E441}"/>
+    <hyperlink ref="K10" r:id="rId14" xr:uid="{B6494471-821E-4BA0-B1F8-79C45FD043BE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId8"/>
-  <drawing r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
+  <drawing r:id="rId16"/>
   <webPublishItems count="1">
     <webPublishItem id="28008" divId="BOM_Electronics_28008" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_Electronics.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId10"/>
+    <tablePart r:id="rId17"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Revised Sources for Thermal Protections
</commit_message>
<xml_diff>
--- a/bom/BOM_Electronics.xlsx
+++ b/bom/BOM_Electronics.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A226B76-504E-4DF1-8DB5-1E24A245967B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A1715B-D5CB-492E-8CAB-FFB3AE369991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{1A685599-6F45-4184-BD49-3F7235A0E362}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21820" xr2:uid="{1A685599-6F45-4184-BD49-3F7235A0E362}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -145,16 +145,7 @@
     <t>Thermostat 150C</t>
   </si>
   <si>
-    <t>Thermal Cut-Off 184C</t>
-  </si>
-  <si>
-    <t>TCO 250VAC 10A 184C</t>
-  </si>
-  <si>
     <t>1*</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/en/products/detail/cantherm/SDF-DF184S/1014767</t>
   </si>
   <si>
     <t>Sensors</t>
@@ -259,11 +250,6 @@
   <si>
     <t>This NC (normally closed) thermostat will open the circuit and cut the power to the bed heat pad incase the bed plate reaches over 150C. You can select other models with higher values if you intend to print with higher bed temperature.
 This Thermostat acts as a safety measure in case of controller or SSR fault.</t>
-  </si>
-  <si>
-    <t>*Optional.
-This thermal fuse can be added to the heat bed circuit and mounted under the bed to provide an additional level of safety against potential heater control jam.
-In case the Control Board, The SSR and the Thermal switch have failed to cut power to the heater pad, this device will permanently open the circuit at 184C. Its internal will melt.</t>
   </si>
   <si>
     <t>*Already Included into Selected Print Head BOM.
@@ -413,6 +399,20 @@
   </si>
   <si>
     <t>Fysetc S6 Spider V1.1</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/en/products/detail/cantherm/SDF-DF192S/1014768</t>
+  </si>
+  <si>
+    <t>TCO 250VAC 10A 192C</t>
+  </si>
+  <si>
+    <t>Thermal Cut-Off 192C</t>
+  </si>
+  <si>
+    <t>*Optional.
+This thermal fuse can be added to the heat bed circuit and mounted under the bed to provide an additional level of safety against potential heater control jam.
+In case the Control Board, The SSR and the Thermal switch have failed to cut power to the heater pad, this device will permanently open the circuit at 192C. Its internal will melt.</t>
   </si>
 </sst>
 </file>
@@ -698,7 +698,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -751,9 +751,6 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -784,13 +781,13 @@
     <xf numFmtId="0" fontId="8" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -817,7 +814,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -826,7 +823,7 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2721,25 +2718,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4DA158D-DB07-4293-994E-A3724E044295}">
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" customWidth="1"/>
-    <col min="2" max="2" width="22.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.54296875" customWidth="1"/>
+    <col min="2" max="2" width="22.81640625" customWidth="1"/>
     <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="4" max="4" width="24.54296875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
-    <col min="6" max="6" width="27.5703125" customWidth="1"/>
-    <col min="7" max="7" width="17.140625" customWidth="1"/>
-    <col min="9" max="9" width="56.140625" customWidth="1"/>
+    <col min="6" max="6" width="27.54296875" customWidth="1"/>
+    <col min="7" max="7" width="17.1796875" customWidth="1"/>
+    <col min="9" max="9" width="56.1796875" customWidth="1"/>
     <col min="10" max="10" width="24" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="56.5703125" customWidth="1"/>
+    <col min="11" max="11" width="56.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="8" customFormat="1" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" s="8" customFormat="1" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2774,24 +2771,24 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="8" customFormat="1" ht="23.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="36" t="s">
-        <v>58</v>
-      </c>
-      <c r="B2" s="37" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="38"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="41"/>
+    <row r="2" spans="1:11" s="8" customFormat="1" ht="23.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="36" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="37"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="36"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="40"/>
     </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="8" customFormat="1" ht="111.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="9" t="s">
         <v>12</v>
       </c>
@@ -2799,7 +2796,7 @@
         <v>13</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D3"/>
       <c r="E3" s="12" t="s">
@@ -2815,7 +2812,7 @@
         <v>1</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J3" s="16" t="s">
         <v>15</v>
@@ -2824,593 +2821,593 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="8" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:11" s="8" customFormat="1" ht="111.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="21" t="s">
-        <v>50</v>
+      <c r="C4" s="20" t="s">
+        <v>47</v>
       </c>
       <c r="D4"/>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="21" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="21" t="s">
         <v>19</v>
       </c>
       <c r="G4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H4" s="23">
+      <c r="H4" s="22">
         <v>1</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J4" s="16" t="s">
         <v>15</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="25" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:11" s="8" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="19" t="s">
+    <row r="5" spans="1:11" s="8" customFormat="1" ht="170.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D5"/>
       <c r="E5" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F5" s="12" t="s">
-        <v>97</v>
-      </c>
-      <c r="G5" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="G5" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="J5" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K5" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="36" t="s">
-        <v>59</v>
-      </c>
-      <c r="B6" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="C6" s="28"/>
-      <c r="D6" s="29"/>
-      <c r="E6" s="30"/>
-      <c r="F6" s="30"/>
-      <c r="G6" s="31"/>
-      <c r="H6" s="32"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="34"/>
-      <c r="K6" s="35"/>
+    <row r="6" spans="1:11" s="8" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A6" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="41" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="27"/>
+      <c r="D6" s="28"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="29"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="31"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="33"/>
+      <c r="K6" s="34"/>
     </row>
-    <row r="7" spans="1:11" s="8" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="19" t="s">
+    <row r="7" spans="1:11" s="8" customFormat="1" ht="111.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>48</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>51</v>
       </c>
       <c r="D7"/>
       <c r="E7" s="12" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="F7" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="G7" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="14">
         <v>1</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="J7" s="16" t="s">
         <v>15</v>
       </c>
       <c r="K7" s="17" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="8" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="19" t="s">
+    <row r="8" spans="1:11" s="8" customFormat="1" ht="170.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="D8"/>
       <c r="E8" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F8" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G8" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G8" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="J8" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K8" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="36" t="s">
+    <row r="9" spans="1:11" s="8" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A9" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="B9" s="44" t="s">
-        <v>100</v>
-      </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="29"/>
-      <c r="E9" s="30"/>
-      <c r="F9" s="30"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32"/>
-      <c r="I9" s="33"/>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="28"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="29"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="32"/>
+      <c r="J9" s="33"/>
+      <c r="K9" s="34"/>
     </row>
-    <row r="10" spans="1:11" s="8" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="19" t="s">
+    <row r="10" spans="1:11" s="8" customFormat="1" ht="170.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A10" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="D10"/>
       <c r="E10" s="12" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="F10" s="12"/>
-      <c r="G10" s="18"/>
+      <c r="G10" s="13"/>
       <c r="H10" s="14"/>
       <c r="I10" s="15"/>
       <c r="J10" s="16"/>
       <c r="K10" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="8" customFormat="1" ht="170.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="19" t="s">
+    <row r="11" spans="1:11" s="8" customFormat="1" ht="170.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D11"/>
       <c r="E11" s="12" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="F11" s="12" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G11" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H11" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K11" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="8" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="36" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="30"/>
-      <c r="F12" s="30"/>
-      <c r="G12" s="31"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="33"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="35"/>
+    <row r="12" spans="1:11" s="8" customFormat="1" ht="18.5" x14ac:dyDescent="0.35">
+      <c r="A12" s="35" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" s="26"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="31"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="33"/>
+      <c r="K12" s="34"/>
     </row>
-    <row r="13" spans="1:11" s="8" customFormat="1" ht="111.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="19" t="s">
+    <row r="13" spans="1:11" s="8" customFormat="1" ht="111.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="20" t="s">
+      <c r="B13" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="C13" s="21">
+      <c r="C13" s="20">
         <v>3</v>
       </c>
       <c r="D13"/>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="21" t="s">
         <v>23</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="23">
+      <c r="H13" s="22">
         <v>1</v>
       </c>
-      <c r="I13" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="J13" s="25" t="s">
+      <c r="I13" s="23" t="s">
+        <v>65</v>
+      </c>
+      <c r="J13" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K13" s="26" t="s">
-        <v>86</v>
+      <c r="K13" s="25" t="s">
+        <v>82</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="8" customFormat="1" ht="116.1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="19" t="s">
+    <row r="14" spans="1:11" s="8" customFormat="1" ht="116.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B14" s="20" t="s">
-        <v>62</v>
+      <c r="B14" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="C14" s="11">
         <v>4</v>
       </c>
       <c r="D14"/>
       <c r="E14" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="18"/>
+        <v>62</v>
+      </c>
+      <c r="G14" s="13"/>
       <c r="H14" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="J14" s="16" t="s">
-        <v>64</v>
-      </c>
-      <c r="K14" s="43" t="s">
-        <v>89</v>
+        <v>61</v>
+      </c>
+      <c r="K14" s="42" t="s">
+        <v>85</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="157.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="19" t="s">
+    <row r="15" spans="1:11" ht="155" x14ac:dyDescent="0.35">
+      <c r="A15" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B15" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="21">
+      <c r="B15" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C15" s="20">
         <v>5</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="21" t="s">
         <v>25</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="23">
+      <c r="H15" s="22">
         <v>1</v>
       </c>
-      <c r="I15" s="24" t="s">
-        <v>87</v>
-      </c>
-      <c r="J15" s="25" t="s">
+      <c r="I15" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K15" s="26" t="s">
-        <v>88</v>
+      <c r="K15" s="25" t="s">
+        <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="19" t="s">
+    <row r="16" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B16" s="20" t="s">
-        <v>62</v>
+      <c r="B16" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="C16" s="11">
         <v>6</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="21" t="s">
         <v>27</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="23">
+      <c r="H16" s="22">
         <v>1</v>
       </c>
-      <c r="I16" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="J16" s="25" t="s">
+      <c r="I16" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="J16" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K16" s="26" t="s">
-        <v>91</v>
+      <c r="K16" s="25" t="s">
+        <v>87</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="19" t="s">
+    <row r="17" spans="1:11" ht="90" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B17" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C17" s="21">
+      <c r="B17" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C17" s="20">
         <v>7</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H17" s="23">
+      <c r="H17" s="22">
         <v>1</v>
       </c>
-      <c r="I17" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="J17" s="25" t="s">
+      <c r="I17" s="23" t="s">
+        <v>67</v>
+      </c>
+      <c r="J17" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="K17" s="26" t="s">
-        <v>94</v>
+      <c r="K17" s="25" t="s">
+        <v>90</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="126" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+    <row r="18" spans="1:11" ht="108.5" x14ac:dyDescent="0.35">
+      <c r="A18" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="20" t="s">
-        <v>62</v>
+      <c r="B18" s="19" t="s">
+        <v>59</v>
       </c>
       <c r="C18" s="11">
         <v>8</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H18" s="23">
+      <c r="H18" s="22">
         <v>1</v>
       </c>
-      <c r="I18" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="J18" s="25" t="s">
+      <c r="I18" s="23" t="s">
+        <v>68</v>
+      </c>
+      <c r="J18" s="24" t="s">
         <v>33</v>
       </c>
-      <c r="K18" s="26" t="s">
+      <c r="K18" s="25" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="138.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="19" t="s">
+    <row r="19" spans="1:11" ht="138.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="C19" s="21">
+      <c r="B19" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="C19" s="20">
         <v>9</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="F19" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="G19" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H19" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="J19" s="24" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="25" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="133" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20" s="19" t="s">
         <v>36</v>
-      </c>
-      <c r="F19" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H19" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="J19" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="26" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" ht="132.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="19" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="20" t="s">
-        <v>39</v>
       </c>
       <c r="C20" s="11">
         <v>10</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="21" t="s">
+        <v>37</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="13" t="s">
+        <v>11</v>
+      </c>
+      <c r="H20" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="I20" s="23" t="s">
+        <v>69</v>
+      </c>
+      <c r="J20" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="K20" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="C21" s="20">
+        <v>11</v>
+      </c>
+      <c r="E21" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F21" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G21" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="H20" s="23" t="s">
-        <v>37</v>
-      </c>
-      <c r="I20" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="J20" s="25" t="s">
+      <c r="H21" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="K20" s="26" t="s">
-        <v>82</v>
+      <c r="I21" s="23" t="s">
+        <v>43</v>
+      </c>
+      <c r="J21" s="24" t="s">
+        <v>44</v>
+      </c>
+      <c r="K21" s="25" t="s">
+        <v>91</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="19" t="s">
+    <row r="22" spans="1:11" ht="81.650000000000006" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B21" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="C21" s="21">
-        <v>11</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>43</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>44</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="I21" s="24" t="s">
-        <v>46</v>
-      </c>
-      <c r="J21" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="K21" s="26" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="81.599999999999994" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="19" t="s">
-        <v>12</v>
-      </c>
       <c r="B22" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C22" s="11">
         <v>12</v>
       </c>
       <c r="E22" s="12" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="F22" s="12" t="s">
-        <v>83</v>
-      </c>
-      <c r="G22" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="G22" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H22" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I22" s="15" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="J22" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K22" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="84.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="19" t="s">
+    <row r="23" spans="1:11" ht="85" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A23" s="18" t="s">
         <v>12</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C23" s="11">
         <v>13</v>
       </c>
       <c r="E23" s="12" t="s">
+        <v>76</v>
+      </c>
+      <c r="F23" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F23" s="12" t="s">
-        <v>84</v>
-      </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="13" t="s">
         <v>11</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="I23" s="15" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="K23" s="17" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -3429,15 +3426,16 @@
     <hyperlink ref="K5" r:id="rId12" xr:uid="{D54CB7AA-26E4-4CE6-B722-81FA3F21507D}"/>
     <hyperlink ref="K11" r:id="rId13" xr:uid="{21EBD8DB-10FC-4A97-A28E-DC53AEE9E441}"/>
     <hyperlink ref="K10" r:id="rId14" xr:uid="{B6494471-821E-4BA0-B1F8-79C45FD043BE}"/>
+    <hyperlink ref="K18" r:id="rId15" xr:uid="{782212B0-3CCE-4C66-9E18-4ED441B54BFF}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId15"/>
-  <drawing r:id="rId16"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId16"/>
+  <drawing r:id="rId17"/>
   <webPublishItems count="1">
     <webPublishItem id="28008" divId="BOM_Electronics_28008" sourceType="sheet" destinationFile="C:\Users\olivi\OneDrive\Documents\GitHub\HevORT\bom\BOM_Electronics.htm" autoRepublish="1"/>
   </webPublishItems>
   <tableParts count="1">
-    <tablePart r:id="rId17"/>
+    <tablePart r:id="rId18"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>